<commit_message>
Modify program to find data of all date range in April
</commit_message>
<xml_diff>
--- a/Monitors.xlsx
+++ b/Monitors.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,10 +388,94 @@
         <v>No. Of Monitors</v>
       </c>
       <c r="C1" t="str">
+        <v>04/01/2020</v>
+      </c>
+      <c r="D1" t="str">
+        <v>04/02/2020</v>
+      </c>
+      <c r="E1" t="str">
+        <v>04/03/2020</v>
+      </c>
+      <c r="F1" t="str">
+        <v>04/04/2020</v>
+      </c>
+      <c r="G1" t="str">
+        <v>04/05/2020</v>
+      </c>
+      <c r="H1" t="str">
+        <v>04/06/2020</v>
+      </c>
+      <c r="I1" t="str">
+        <v>04/07/2020</v>
+      </c>
+      <c r="J1" t="str">
+        <v>04/08/2020</v>
+      </c>
+      <c r="K1" t="str">
+        <v>04/09/2020</v>
+      </c>
+      <c r="L1" t="str">
+        <v>04/10/2020</v>
+      </c>
+      <c r="M1" t="str">
+        <v>04/11/2020</v>
+      </c>
+      <c r="N1" t="str">
+        <v>04/12/2020</v>
+      </c>
+      <c r="O1" t="str">
+        <v>04/13/2020</v>
+      </c>
+      <c r="P1" t="str">
+        <v>04/14/2020</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>04/15/2020</v>
+      </c>
+      <c r="R1" t="str">
+        <v>04/16/2020</v>
+      </c>
+      <c r="S1" t="str">
+        <v>04/17/2020</v>
+      </c>
+      <c r="T1" t="str">
+        <v>04/18/2020</v>
+      </c>
+      <c r="U1" t="str">
+        <v>04/19/2020</v>
+      </c>
+      <c r="V1" t="str">
+        <v>04/20/2020</v>
+      </c>
+      <c r="W1" t="str">
+        <v>04/21/2020</v>
+      </c>
+      <c r="X1" t="str">
         <v>04/22/2020</v>
       </c>
-      <c r="D1" t="str">
+      <c r="Y1" t="str">
+        <v>04/23/2020</v>
+      </c>
+      <c r="Z1" t="str">
         <v>04/24/2020</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>04/25/2020</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>04/26/2020</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>04/27/2020</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>04/28/2020</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>04/29/2020</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>04/30/2020</v>
       </c>
     </row>
     <row r="2">
@@ -402,15 +486,99 @@
         <v>6</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
         <v>23</v>
       </c>
-      <c r="D2">
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <v>161</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AF2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>